<commit_message>
Tableau check list des problemes
</commit_message>
<xml_diff>
--- a/P4_analyse_by_shehzad.xlsx
+++ b/P4_analyse_by_shehzad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bureau\Desktop\P4_shehzad_qaiser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E8E344-B2EA-4BA3-BAA7-D71E07302FDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AF1438-C5E4-4C3F-B9F4-480EC1765A1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18690" windowHeight="9135" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="235">
   <si>
     <t>URL :</t>
   </si>
@@ -122,12 +122,6 @@
   </si>
   <si>
     <t>Présence de liens spammy ?</t>
-  </si>
-  <si>
-    <t>Categorie</t>
-  </si>
-  <si>
-    <t>Problème analysé</t>
   </si>
   <si>
     <t>Bonne pratique à adopter</t>
@@ -650,12 +644,126 @@
   <si>
     <t xml:space="preserve">Teste l'accessibilité avec Tanaguru </t>
   </si>
+  <si>
+    <t>La checklist pour renforcer son SEO on-site</t>
+  </si>
+  <si>
+    <t>Les « classiques » du SEO à réaliser en priorité</t>
+  </si>
+  <si>
+    <t>2) Vérifiez que toutes vos pages ont une balise META &lt;title&gt; qui ne dépasse pas 65 caractères idéalement.</t>
+  </si>
+  <si>
+    <t>3) Rédigez des balises META &lt;description&gt; entre 70 et 320 caractères qui donnent envie aux internautes de cliquer.</t>
+  </si>
+  <si>
+    <t>4) Vos URLs doivent être compréhensibles par un humain, et idéalement ne dépassent pas 115 caractères.</t>
+  </si>
+  <si>
+    <t>Votre contenu à proprement dit</t>
+  </si>
+  <si>
+    <t>5) Rédigez des contenus de plus de 500 mots, voire encore plus longs si vous le pouvez (la longueur du texte compte pour votre référencement).</t>
+  </si>
+  <si>
+    <t>6) Utilisez les mots justes et un vocabulaire riche dans vos contenus pour maximiser votre impact SEO (aidez vous d’un outil).</t>
+  </si>
+  <si>
+    <t>7) Utilisez des images dans vos contenus, en prenant soin de renseigner les balises &lt;alt&gt; et &lt;title&gt; de vos visuels.</t>
+  </si>
+  <si>
+    <t>8) Prenez soins de garder la taille de vos images la plus légère possible pour ne pas impacter défavorablement votre temps de chargement.</t>
+  </si>
+  <si>
+    <t>9) « Stratégisez » votre maillage interne en utilisant un outil comme Google Search Console.</t>
+  </si>
+  <si>
+    <t>Soigner la structuration HTML</t>
+  </si>
+  <si>
+    <t>10) Structurez votre contenu avec des titres H1 – H6.</t>
+  </si>
+  <si>
+    <t>11) Si vous avez un contenu qui se lit sur plusieurs pages, utilisez les balises de pagination rel= »next » et rel= »prev ».</t>
+  </si>
+  <si>
+    <t>12) Si votre contenu s’y prête, n’oubliez pas d’ajouter toutes les micro-données possibles  (voir schema.org).</t>
+  </si>
+  <si>
+    <t>13) Votre contenu texte doit idéalement représenter plus de 10% de votre code HTML.</t>
+  </si>
+  <si>
+    <t>L’expérience utilisateur a aussi un impact SEO</t>
+  </si>
+  <si>
+    <t>15) Assurez-vous que votre site est compatible avec les appareils mobiles et évitez les erreurs UX basiques d’un site mobile.</t>
+  </si>
+  <si>
+    <t>16) Assurez vous de garder une page légère, pour favoriser un temps de chargement rapide.</t>
+  </si>
+  <si>
+    <t>17) Corrigez toutes les erreurs d’exploitation, et faites la chasse aux pages 404.</t>
+  </si>
+  <si>
+    <t>18) Déliez tous les liens cassés qui peuvent être présents sur votre site.</t>
+  </si>
+  <si>
+    <t>19) Ajoutez une Favicon à votre site, qui apparaisse sur tous les navigateurs.</t>
+  </si>
+  <si>
+    <t>20) Ne pensez pas qu’aux moteurs de recherche et cherchez à développer une vraie marque sur la toile pour gagner la bataille du « préférencement ».</t>
+  </si>
+  <si>
+    <t>Les éléments techniques SEO à prendre en compte</t>
+  </si>
+  <si>
+    <t>21) Assurez-vous d’avoir un sitemap XML</t>
+  </si>
+  <si>
+    <t>23) Eviter que les éventuels paramètres de vos URLs (ex: quand vous filtrez un catalogue produit) génèrent du duplicate content, ou cannibalisent le SEO d’autres pages.</t>
+  </si>
+  <si>
+    <t>24) De manière générale, évitez les techniques de cloaking (servir un contenu différent aux moteurs de recherche et aux utilisateurs)</t>
+  </si>
+  <si>
+    <t>25) Passez au protocole HTTPs (tout en évitant ses pièges SEO)</t>
+  </si>
+  <si>
+    <t>5. CHECK LIST SEO</t>
+  </si>
+  <si>
+    <t>d’une en-tête HTTP X-Robots-Tag ou d’une indication de non indexation dans votre fichier robot.txt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Assurez vous que l‘indexation de vos pages n’est pas bloquée à cause d’une balise NoIndex, </t>
+  </si>
+  <si>
+    <t>pour essayer d’influencer votre classement dans les moteurs de recherche.</t>
+  </si>
+  <si>
+    <t>14) N’utilisez pas de liens ou de textes cachés (par exemple un texte blanc sur fond blanc) au risque que Google considère la manœuvre comme une tentative malhonnête</t>
+  </si>
+  <si>
+    <t>Utilisez une balise &lt;canonical&gt; pour déclarer quelle variante vous voulez voir dans les résultats de recherche.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22) Évitez le duplicate content « bête » à cause des deux variantes de votre site, avec ou sans les « www » (par exemple, http://www.monsite.com et http://monsite.com). </t>
+  </si>
+  <si>
+    <t>N°</t>
+  </si>
+  <si>
+    <t>Problèmes analysés</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -767,8 +875,14 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -838,6 +952,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -972,7 +1104,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
@@ -1034,26 +1166,41 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1096,37 +1243,44 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1138,6 +1292,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFFCC"/>
       <color rgb="FFCC66FF"/>
       <color rgb="FF00CC99"/>
       <color rgb="FF00CCFF"/>
@@ -1158,7 +1313,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>249382</xdr:rowOff>
@@ -1480,37 +1635,37 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:L109"/>
+  <dimension ref="A1:L169"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" style="71"/>
+    <col min="1" max="1" width="10.88671875" style="51"/>
     <col min="2" max="2" width="21.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="10.88671875" style="1"/>
     <col min="6" max="6" width="16.88671875" style="1" customWidth="1"/>
     <col min="7" max="10" width="10.88671875" style="1"/>
-    <col min="11" max="11" width="58.5546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.88671875" style="71"/>
+    <col min="11" max="11" width="66.77734375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.88671875" style="51"/>
     <col min="13" max="16384" width="10.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
       <c r="D1" s="39"/>
       <c r="E1" s="37"/>
       <c r="F1" s="40" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G1" s="38"/>
       <c r="H1" s="38"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="74"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="54"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B2" s="41"/>
@@ -1529,215 +1684,212 @@
       <c r="K3" s="45"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="49" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2"/>
       <c r="K4" s="45"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="70"/>
+      <c r="B5" s="50"/>
       <c r="K5" s="45"/>
     </row>
     <row r="6" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="49" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K6" s="45"/>
     </row>
     <row r="7" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="70"/>
+      <c r="B7" s="50"/>
       <c r="K7" s="45"/>
     </row>
     <row r="8" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="69" t="s">
+      <c r="B8" s="49" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K8" s="45"/>
     </row>
     <row r="9" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="70"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K9" s="45"/>
     </row>
     <row r="10" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="70"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K10" s="45"/>
     </row>
     <row r="11" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="69" t="s">
+      <c r="B11" s="50"/>
+      <c r="K11" s="45"/>
+    </row>
+    <row r="12" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="53" t="s">
+      <c r="C12" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="K11" s="45"/>
-    </row>
-    <row r="12" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="54"/>
-      <c r="C12" s="53" t="s">
-        <v>156</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>192</v>
+        <v>163</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="K12" s="45"/>
     </row>
     <row r="13" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="42"/>
-      <c r="C13" s="53" t="s">
-        <v>157</v>
+      <c r="B13" s="48"/>
+      <c r="C13" s="47" t="s">
+        <v>154</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="K13" s="45"/>
     </row>
     <row r="14" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="42"/>
-      <c r="C14" s="53" t="s">
-        <v>158</v>
+      <c r="C14" s="47" t="s">
+        <v>155</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="K14" s="45"/>
     </row>
     <row r="15" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="42"/>
-      <c r="C15" s="53" t="s">
-        <v>196</v>
+      <c r="C15" s="47" t="s">
+        <v>156</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="K15" s="45"/>
     </row>
     <row r="16" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="42"/>
-      <c r="C16" s="53" t="s">
-        <v>198</v>
+      <c r="C16" s="47" t="s">
+        <v>194</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="K16" s="45"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="42"/>
-      <c r="C17" s="53" t="s">
-        <v>167</v>
+      <c r="C17" s="47" t="s">
+        <v>196</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>159</v>
+        <v>195</v>
       </c>
       <c r="K17" s="45"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="42"/>
-      <c r="C18" s="53" t="s">
-        <v>160</v>
+      <c r="C18" s="47" t="s">
+        <v>165</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="K18" s="45"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="42"/>
-      <c r="C19" s="53" t="s">
-        <v>190</v>
+      <c r="C19" s="47" t="s">
+        <v>158</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>191</v>
+        <v>159</v>
       </c>
       <c r="K19" s="45"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="42"/>
-      <c r="C20" s="53" t="s">
+      <c r="C20" s="47" t="s">
+        <v>188</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="K20" s="45"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="42"/>
-      <c r="C21" s="53" t="s">
-        <v>174</v>
+      <c r="C21" s="47" t="s">
+        <v>187</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="K21" s="45"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="42"/>
-      <c r="C22" s="53"/>
+      <c r="C22" s="47" t="s">
+        <v>172</v>
+      </c>
       <c r="G22" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="K22" s="45"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="42"/>
-      <c r="C23" s="53" t="s">
+      <c r="C23" s="47"/>
+      <c r="G23" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="K23" s="45"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="42"/>
-      <c r="C24" s="53" t="s">
+      <c r="C24" s="47" t="s">
         <v>171</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K24" s="45"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="42"/>
-      <c r="C25" s="53" t="s">
-        <v>177</v>
+      <c r="C25" s="47" t="s">
+        <v>169</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="K25" s="45"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="42"/>
-      <c r="C26" s="53"/>
+      <c r="C26" s="47" t="s">
+        <v>175</v>
+      </c>
       <c r="G26" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="K26" s="45"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" s="42"/>
+      <c r="C27" s="47"/>
       <c r="G27" s="1" t="s">
         <v>176</v>
       </c>
@@ -1745,77 +1897,72 @@
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" s="42"/>
-      <c r="C28" s="53" t="s">
-        <v>180</v>
-      </c>
       <c r="G28" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="K28" s="45"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" s="42"/>
-      <c r="C29" s="53" t="s">
-        <v>181</v>
+      <c r="C29" s="47" t="s">
+        <v>178</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="K29" s="45"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" s="42"/>
+      <c r="C30" s="47" t="s">
+        <v>179</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>180</v>
+      </c>
       <c r="K30" s="45"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B31" s="43"/>
-      <c r="K31" s="46"/>
-    </row>
-    <row r="32" spans="2:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="B32" s="55" t="s">
-        <v>183</v>
-      </c>
-      <c r="C32" s="56"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="56"/>
-      <c r="G32" s="56"/>
-      <c r="H32" s="56"/>
-      <c r="I32" s="56"/>
-      <c r="J32" s="56"/>
-      <c r="K32" s="56"/>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B33" s="5" t="s">
+      <c r="B31" s="42"/>
+      <c r="K31" s="45"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B32" s="43"/>
+      <c r="K32" s="46"/>
+    </row>
+    <row r="33" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="B33" s="62" t="s">
+        <v>181</v>
+      </c>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="63"/>
+      <c r="K33" s="63"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B34" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B34" s="3"/>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B35" s="3"/>
+      <c r="C35" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="8"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B35" s="4"/>
-      <c r="C35" s="7"/>
       <c r="D35" s="8"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -1826,36 +1973,36 @@
       <c r="K35" s="4"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="4"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B37" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B37" s="3"/>
-      <c r="C37" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B38" s="4"/>
-      <c r="C38" s="7"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="7" t="s">
+        <v>96</v>
+      </c>
       <c r="D38" s="8"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
@@ -1866,37 +2013,35 @@
       <c r="K38" s="4"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="4"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B40" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B40" s="3"/>
-      <c r="C40" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="D40" s="8"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B41" s="4"/>
+      <c r="B41" s="3"/>
       <c r="C41" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="4"/>
@@ -1908,37 +2053,37 @@
       <c r="K41" s="4"/>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="4"/>
+      <c r="C42" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D42" s="8"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B43" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B43" s="3"/>
-      <c r="C43" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" s="8"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B44" s="3"/>
       <c r="C44" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="4"/>
@@ -1952,7 +2097,7 @@
     <row r="45" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B45" s="3"/>
       <c r="C45" s="7" t="s">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="D45" s="8"/>
       <c r="E45" s="4"/>
@@ -1965,8 +2110,10 @@
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B46" s="3"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
+      <c r="C46" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D46" s="8"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -1976,90 +2123,90 @@
       <c r="K46" s="4"/>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="3"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B48" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="6"/>
-    </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B48" s="3"/>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
+      <c r="K48" s="6"/>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B49" s="3"/>
+      <c r="C49" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D48" s="8"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B49" s="9"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
-      <c r="H49" s="10"/>
-      <c r="I49" s="10"/>
-      <c r="J49" s="10"/>
-      <c r="K49" s="10"/>
-    </row>
-    <row r="51" spans="2:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="B51" s="57" t="s">
-        <v>184</v>
-      </c>
-      <c r="C51" s="58"/>
-      <c r="D51" s="58"/>
-      <c r="E51" s="58"/>
-      <c r="F51" s="58"/>
-      <c r="G51" s="58"/>
-      <c r="H51" s="58"/>
-      <c r="I51" s="58"/>
-      <c r="J51" s="58"/>
-      <c r="K51" s="58"/>
-    </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B52" s="13" t="s">
+      <c r="D49" s="8"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B50" s="9"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
+      <c r="K50" s="10"/>
+    </row>
+    <row r="52" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="B52" s="64" t="s">
+        <v>182</v>
+      </c>
+      <c r="C52" s="65"/>
+      <c r="D52" s="65"/>
+      <c r="E52" s="65"/>
+      <c r="F52" s="65"/>
+      <c r="G52" s="65"/>
+      <c r="H52" s="65"/>
+      <c r="I52" s="65"/>
+      <c r="J52" s="65"/>
+      <c r="K52" s="65"/>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B53" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14"/>
-    </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B53" s="12"/>
-      <c r="C53" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D53" s="12"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="12"/>
-      <c r="I53" s="12"/>
-      <c r="J53" s="12"/>
-      <c r="K53" s="12"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="14"/>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
+      <c r="C54" s="15" t="s">
+        <v>15</v>
+      </c>
       <c r="D54" s="12"/>
       <c r="E54" s="16"/>
       <c r="F54" s="12"/>
@@ -2070,88 +2217,88 @@
       <c r="K54" s="12"/>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B55" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
-      <c r="K55" s="14"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="12"/>
+      <c r="K55" s="12"/>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
-      <c r="J56" s="12"/>
-      <c r="K56" s="12"/>
+      <c r="B56" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
+      <c r="K56" s="14"/>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B57" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
-      <c r="K57" s="14"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="12"/>
+      <c r="K57" s="12"/>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B58" s="12"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="16"/>
-      <c r="F58" s="12"/>
-      <c r="G58" s="12"/>
-      <c r="H58" s="12"/>
-      <c r="I58" s="12"/>
-      <c r="J58" s="12"/>
-      <c r="K58" s="12"/>
+      <c r="B58" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="14"/>
+      <c r="K58" s="14"/>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B59" s="13" t="s">
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="12"/>
+      <c r="J59" s="12"/>
+      <c r="K59" s="12"/>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B60" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
-      <c r="J59" s="14"/>
-      <c r="K59" s="14"/>
-    </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B60" s="12"/>
-      <c r="C60" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D60" s="12"/>
-      <c r="E60" s="16"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
-      <c r="H60" s="12"/>
-      <c r="I60" s="12"/>
-      <c r="J60" s="12"/>
-      <c r="K60" s="12"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="14"/>
+      <c r="J60" s="14"/>
+      <c r="K60" s="14"/>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B61" s="12"/>
-      <c r="C61" s="15"/>
+      <c r="C61" s="15" t="s">
+        <v>17</v>
+      </c>
       <c r="D61" s="12"/>
       <c r="E61" s="16"/>
       <c r="F61" s="12"/>
@@ -2162,63 +2309,61 @@
       <c r="K61" s="12"/>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B62" s="13" t="s">
+      <c r="B62" s="12"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="12"/>
+      <c r="K62" s="12"/>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B63" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
-      <c r="H62" s="14"/>
-      <c r="I62" s="14"/>
-      <c r="J62" s="14"/>
-      <c r="K62" s="14"/>
-    </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B63" s="12"/>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="12"/>
-      <c r="H63" s="12"/>
-      <c r="I63" s="12"/>
-      <c r="J63" s="12"/>
-      <c r="K63" s="12"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
+      <c r="J63" s="14"/>
+      <c r="K63" s="14"/>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B64" s="13" t="s">
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="12"/>
+      <c r="J64" s="12"/>
+      <c r="K64" s="12"/>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B65" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="14"/>
-      <c r="G64" s="14"/>
-      <c r="H64" s="14"/>
-      <c r="I64" s="14"/>
-      <c r="J64" s="14"/>
-      <c r="K64" s="14"/>
-    </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B65" s="12"/>
-      <c r="C65" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="D65" s="12"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="12"/>
-      <c r="G65" s="12"/>
-      <c r="H65" s="12"/>
-      <c r="I65" s="12"/>
-      <c r="J65" s="12"/>
-      <c r="K65" s="12"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
+      <c r="J65" s="14"/>
+      <c r="K65" s="14"/>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B66" s="12"/>
       <c r="C66" s="15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D66" s="12"/>
       <c r="E66" s="16"/>
@@ -2230,37 +2375,37 @@
       <c r="K66" s="12"/>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B67" s="13" t="s">
+      <c r="B67" s="12"/>
+      <c r="C67" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D67" s="12"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="12"/>
+      <c r="I67" s="12"/>
+      <c r="J67" s="12"/>
+      <c r="K67" s="12"/>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B68" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C67" s="17"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
-      <c r="I67" s="14"/>
-      <c r="J67" s="14"/>
-      <c r="K67" s="14"/>
-    </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B68" s="12"/>
-      <c r="C68" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="D68" s="12"/>
-      <c r="E68" s="12"/>
-      <c r="F68" s="12"/>
-      <c r="G68" s="12"/>
-      <c r="H68" s="12"/>
-      <c r="I68" s="12"/>
-      <c r="J68" s="12"/>
-      <c r="K68" s="12"/>
+      <c r="C68" s="17"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="14"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="14"/>
+      <c r="J68" s="14"/>
+      <c r="K68" s="14"/>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B69" s="12"/>
       <c r="C69" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D69" s="12"/>
       <c r="E69" s="12"/>
@@ -2274,10 +2419,10 @@
     <row r="70" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B70" s="12"/>
       <c r="C70" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D70" s="12"/>
-      <c r="E70" s="16"/>
+      <c r="E70" s="12"/>
       <c r="F70" s="12"/>
       <c r="G70" s="12"/>
       <c r="H70" s="12"/>
@@ -2286,37 +2431,37 @@
       <c r="K70" s="12"/>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B71" s="13" t="s">
+      <c r="B71" s="12"/>
+      <c r="C71" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D71" s="12"/>
+      <c r="E71" s="16"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
+      <c r="H71" s="12"/>
+      <c r="I71" s="12"/>
+      <c r="J71" s="12"/>
+      <c r="K71" s="12"/>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B72" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C71" s="14"/>
-      <c r="D71" s="14"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
-      <c r="I71" s="14"/>
-      <c r="J71" s="14"/>
-      <c r="K71" s="14"/>
-    </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B72" s="12"/>
-      <c r="C72" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="D72" s="12"/>
-      <c r="E72" s="16"/>
-      <c r="F72" s="12"/>
-      <c r="G72" s="12"/>
-      <c r="H72" s="12"/>
-      <c r="I72" s="12"/>
-      <c r="J72" s="12"/>
-      <c r="K72" s="12"/>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
+      <c r="I72" s="14"/>
+      <c r="J72" s="14"/>
+      <c r="K72" s="14"/>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B73" s="12"/>
       <c r="C73" s="15" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D73" s="12"/>
       <c r="E73" s="16"/>
@@ -2330,7 +2475,7 @@
     <row r="74" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B74" s="12"/>
       <c r="C74" s="15" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D74" s="12"/>
       <c r="E74" s="16"/>
@@ -2343,7 +2488,9 @@
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B75" s="12"/>
-      <c r="C75" s="15"/>
+      <c r="C75" s="15" t="s">
+        <v>104</v>
+      </c>
       <c r="D75" s="12"/>
       <c r="E75" s="16"/>
       <c r="F75" s="12"/>
@@ -2354,235 +2501,233 @@
       <c r="K75" s="12"/>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B76" s="18" t="s">
+      <c r="B76" s="12"/>
+      <c r="C76" s="15"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="16"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="12"/>
+      <c r="J76" s="12"/>
+      <c r="K76" s="12"/>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B77" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C76" s="14"/>
-      <c r="D76" s="14"/>
-      <c r="E76" s="14"/>
-      <c r="F76" s="14"/>
-      <c r="G76" s="14"/>
-      <c r="H76" s="14"/>
-      <c r="I76" s="14"/>
-      <c r="J76" s="14"/>
-      <c r="K76" s="14"/>
-    </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B77" s="19"/>
-      <c r="C77" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
-      <c r="G77" s="11"/>
-      <c r="H77" s="11"/>
-      <c r="I77" s="11"/>
-      <c r="J77" s="11"/>
-      <c r="K77" s="11"/>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="14"/>
+      <c r="H77" s="14"/>
+      <c r="I77" s="14"/>
+      <c r="J77" s="14"/>
+      <c r="K77" s="14"/>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B78" s="21"/>
-      <c r="C78" s="15"/>
-      <c r="D78" s="12"/>
-      <c r="E78" s="12"/>
-      <c r="F78" s="12"/>
-      <c r="G78" s="12"/>
-      <c r="H78" s="12"/>
-      <c r="I78" s="12"/>
-      <c r="J78" s="12"/>
-      <c r="K78" s="12"/>
+      <c r="B78" s="19"/>
+      <c r="C78" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="11"/>
+      <c r="I78" s="11"/>
+      <c r="J78" s="11"/>
+      <c r="K78" s="11"/>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B79" s="22" t="s">
+      <c r="B79" s="21"/>
+      <c r="C79" s="15"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
+      <c r="H79" s="12"/>
+      <c r="I79" s="12"/>
+      <c r="J79" s="12"/>
+      <c r="K79" s="12"/>
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B80" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C79" s="23"/>
-      <c r="D79" s="24"/>
-      <c r="E79" s="24"/>
-      <c r="F79" s="24"/>
-      <c r="G79" s="24"/>
-      <c r="H79" s="24"/>
-      <c r="I79" s="24"/>
-      <c r="J79" s="24"/>
-      <c r="K79" s="24"/>
-    </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B80" s="25"/>
-      <c r="C80" s="26"/>
-      <c r="D80" s="27"/>
-      <c r="E80" s="27"/>
-      <c r="F80" s="27"/>
-      <c r="G80" s="27"/>
-      <c r="H80" s="27"/>
-      <c r="I80" s="27"/>
-      <c r="J80" s="27"/>
-      <c r="K80" s="27"/>
-    </row>
-    <row r="82" spans="2:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="B82" s="59" t="s">
-        <v>185</v>
-      </c>
-      <c r="C82" s="60"/>
-      <c r="D82" s="60"/>
-      <c r="E82" s="60"/>
-      <c r="F82" s="60"/>
-      <c r="G82" s="60"/>
-      <c r="H82" s="60"/>
-      <c r="I82" s="60"/>
-      <c r="J82" s="60"/>
-      <c r="K82" s="31"/>
-    </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B83" s="63" t="s">
-        <v>145</v>
-      </c>
-      <c r="C83" s="64"/>
-      <c r="D83" s="64"/>
-      <c r="E83" s="64"/>
-      <c r="F83" s="64"/>
-      <c r="G83" s="64"/>
-      <c r="H83" s="64"/>
-      <c r="I83" s="64"/>
-      <c r="J83" s="64"/>
-      <c r="K83" s="64"/>
+      <c r="C80" s="23"/>
+      <c r="D80" s="24"/>
+      <c r="E80" s="24"/>
+      <c r="F80" s="24"/>
+      <c r="G80" s="24"/>
+      <c r="H80" s="24"/>
+      <c r="I80" s="24"/>
+      <c r="J80" s="24"/>
+      <c r="K80" s="24"/>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B81" s="25"/>
+      <c r="C81" s="26"/>
+      <c r="D81" s="27"/>
+      <c r="E81" s="27"/>
+      <c r="F81" s="27"/>
+      <c r="G81" s="27"/>
+      <c r="H81" s="27"/>
+      <c r="I81" s="27"/>
+      <c r="J81" s="27"/>
+      <c r="K81" s="27"/>
+    </row>
+    <row r="83" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="B83" s="66" t="s">
+        <v>183</v>
+      </c>
+      <c r="C83" s="67"/>
+      <c r="D83" s="67"/>
+      <c r="E83" s="67"/>
+      <c r="F83" s="67"/>
+      <c r="G83" s="67"/>
+      <c r="H83" s="67"/>
+      <c r="I83" s="67"/>
+      <c r="J83" s="67"/>
+      <c r="K83" s="31"/>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B84" s="65"/>
-      <c r="C84" s="66"/>
-      <c r="D84" s="66"/>
-      <c r="E84" s="66"/>
-      <c r="F84" s="66"/>
-      <c r="G84" s="66"/>
-      <c r="H84" s="66"/>
-      <c r="I84" s="66"/>
-      <c r="J84" s="66"/>
-      <c r="K84" s="66"/>
+      <c r="B84" s="70" t="s">
+        <v>143</v>
+      </c>
+      <c r="C84" s="71"/>
+      <c r="D84" s="71"/>
+      <c r="E84" s="71"/>
+      <c r="F84" s="71"/>
+      <c r="G84" s="71"/>
+      <c r="H84" s="71"/>
+      <c r="I84" s="71"/>
+      <c r="J84" s="71"/>
+      <c r="K84" s="71"/>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B85" s="65" t="s">
-        <v>107</v>
-      </c>
-      <c r="C85" s="66"/>
-      <c r="D85" s="66"/>
-      <c r="E85" s="66"/>
-      <c r="F85" s="66"/>
-      <c r="G85" s="66"/>
-      <c r="H85" s="66"/>
-      <c r="I85" s="66"/>
-      <c r="J85" s="66"/>
-      <c r="K85" s="66"/>
+      <c r="B85" s="72"/>
+      <c r="C85" s="73"/>
+      <c r="D85" s="73"/>
+      <c r="E85" s="73"/>
+      <c r="F85" s="73"/>
+      <c r="G85" s="73"/>
+      <c r="H85" s="73"/>
+      <c r="I85" s="73"/>
+      <c r="J85" s="73"/>
+      <c r="K85" s="73"/>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B86" s="65" t="s">
+      <c r="B86" s="72" t="s">
+        <v>105</v>
+      </c>
+      <c r="C86" s="73"/>
+      <c r="D86" s="73"/>
+      <c r="E86" s="73"/>
+      <c r="F86" s="73"/>
+      <c r="G86" s="73"/>
+      <c r="H86" s="73"/>
+      <c r="I86" s="73"/>
+      <c r="J86" s="73"/>
+      <c r="K86" s="73"/>
+    </row>
+    <row r="87" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B87" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="C86" s="66"/>
-      <c r="D86" s="66"/>
-      <c r="E86" s="66"/>
-      <c r="F86" s="66"/>
-      <c r="G86" s="66"/>
-      <c r="H86" s="66"/>
-      <c r="I86" s="66"/>
-      <c r="J86" s="66"/>
-      <c r="K86" s="66"/>
-    </row>
-    <row r="87" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B87" s="65"/>
-      <c r="C87" s="66"/>
-      <c r="D87" s="66"/>
-      <c r="E87" s="66"/>
-      <c r="F87" s="66"/>
-      <c r="G87" s="66"/>
-      <c r="H87" s="66"/>
-      <c r="I87" s="66"/>
-      <c r="J87" s="66"/>
-      <c r="K87" s="66"/>
+      <c r="C87" s="73"/>
+      <c r="D87" s="73"/>
+      <c r="E87" s="73"/>
+      <c r="F87" s="73"/>
+      <c r="G87" s="73"/>
+      <c r="H87" s="73"/>
+      <c r="I87" s="73"/>
+      <c r="J87" s="73"/>
+      <c r="K87" s="73"/>
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B88" s="65" t="s">
+      <c r="B88" s="72"/>
+      <c r="C88" s="73"/>
+      <c r="D88" s="73"/>
+      <c r="E88" s="73"/>
+      <c r="F88" s="73"/>
+      <c r="G88" s="73"/>
+      <c r="H88" s="73"/>
+      <c r="I88" s="73"/>
+      <c r="J88" s="73"/>
+      <c r="K88" s="73"/>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B89" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="C88" s="66"/>
-      <c r="D88" s="66"/>
-      <c r="E88" s="66"/>
-      <c r="F88" s="66"/>
-      <c r="G88" s="66"/>
-      <c r="H88" s="66"/>
-      <c r="I88" s="66"/>
-      <c r="J88" s="66"/>
-      <c r="K88" s="66"/>
-    </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B89" s="67" t="s">
+      <c r="C89" s="73"/>
+      <c r="D89" s="73"/>
+      <c r="E89" s="73"/>
+      <c r="F89" s="73"/>
+      <c r="G89" s="73"/>
+      <c r="H89" s="73"/>
+      <c r="I89" s="73"/>
+      <c r="J89" s="73"/>
+      <c r="K89" s="73"/>
+    </row>
+    <row r="90" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B90" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="C89" s="68"/>
-      <c r="D89" s="68"/>
-      <c r="E89" s="68"/>
-      <c r="F89" s="68"/>
-      <c r="G89" s="68"/>
-      <c r="H89" s="68"/>
-      <c r="I89" s="68"/>
-      <c r="J89" s="68"/>
-      <c r="K89" s="68"/>
-    </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B90" s="30" t="s">
+      <c r="C90" s="75"/>
+      <c r="D90" s="75"/>
+      <c r="E90" s="75"/>
+      <c r="F90" s="75"/>
+      <c r="G90" s="75"/>
+      <c r="H90" s="75"/>
+      <c r="I90" s="75"/>
+      <c r="J90" s="75"/>
+      <c r="K90" s="75"/>
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B91" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C90" s="31"/>
-      <c r="D90" s="31"/>
-      <c r="E90" s="31"/>
-      <c r="F90" s="31"/>
-      <c r="G90" s="31"/>
-      <c r="H90" s="31"/>
-      <c r="I90" s="31"/>
-      <c r="J90" s="31"/>
-      <c r="K90" s="31"/>
-    </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B91" s="28"/>
-      <c r="C91" s="29"/>
-      <c r="D91" s="29"/>
-      <c r="E91" s="29"/>
-      <c r="F91" s="29"/>
-      <c r="G91" s="29"/>
-      <c r="H91" s="29"/>
-      <c r="I91" s="29"/>
-      <c r="J91" s="29"/>
-      <c r="K91" s="29"/>
+      <c r="C91" s="31"/>
+      <c r="D91" s="31"/>
+      <c r="E91" s="31"/>
+      <c r="F91" s="31"/>
+      <c r="G91" s="31"/>
+      <c r="H91" s="31"/>
+      <c r="I91" s="31"/>
+      <c r="J91" s="31"/>
+      <c r="K91" s="31"/>
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B92" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="C92" s="31"/>
-      <c r="D92" s="31"/>
-      <c r="E92" s="31"/>
-      <c r="F92" s="31"/>
-      <c r="G92" s="31"/>
-      <c r="H92" s="31"/>
-      <c r="I92" s="31"/>
-      <c r="J92" s="31"/>
-      <c r="K92" s="31"/>
+      <c r="B92" s="28"/>
+      <c r="C92" s="29"/>
+      <c r="D92" s="29"/>
+      <c r="E92" s="29"/>
+      <c r="F92" s="29"/>
+      <c r="G92" s="29"/>
+      <c r="H92" s="29"/>
+      <c r="I92" s="29"/>
+      <c r="J92" s="29"/>
+      <c r="K92" s="29"/>
     </row>
     <row r="93" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B93" s="32"/>
-      <c r="C93" s="33"/>
-      <c r="D93" s="33"/>
-      <c r="E93" s="33"/>
-      <c r="F93" s="33"/>
-      <c r="G93" s="33"/>
-      <c r="H93" s="33"/>
-      <c r="I93" s="33"/>
-      <c r="J93" s="33"/>
-      <c r="K93" s="33"/>
+      <c r="B93" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="C93" s="31"/>
+      <c r="D93" s="31"/>
+      <c r="E93" s="31"/>
+      <c r="F93" s="31"/>
+      <c r="G93" s="31"/>
+      <c r="H93" s="31"/>
+      <c r="I93" s="31"/>
+      <c r="J93" s="31"/>
+      <c r="K93" s="31"/>
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B94" s="32" t="s">
-        <v>28</v>
-      </c>
+      <c r="B94" s="32"/>
       <c r="C94" s="33"/>
       <c r="D94" s="33"/>
       <c r="E94" s="33"/>
@@ -2594,7 +2739,9 @@
       <c r="K94" s="33"/>
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B95" s="32"/>
+      <c r="B95" s="32" t="s">
+        <v>28</v>
+      </c>
       <c r="C95" s="33"/>
       <c r="D95" s="33"/>
       <c r="E95" s="33"/>
@@ -2605,37 +2752,35 @@
       <c r="J95" s="33"/>
       <c r="K95" s="33"/>
     </row>
-    <row r="97" spans="2:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="B97" s="61" t="s">
-        <v>187</v>
-      </c>
-      <c r="C97" s="62"/>
-      <c r="D97" s="62"/>
-      <c r="E97" s="62"/>
-      <c r="F97" s="62"/>
-      <c r="G97" s="62"/>
-      <c r="H97" s="62"/>
-      <c r="I97" s="62"/>
-      <c r="J97" s="62"/>
-      <c r="K97" s="62"/>
-    </row>
-    <row r="98" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B98" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C98" s="35"/>
-      <c r="D98" s="35"/>
-      <c r="E98" s="35"/>
-      <c r="F98" s="35"/>
-      <c r="G98" s="35"/>
-      <c r="H98" s="35"/>
-      <c r="I98" s="35"/>
-      <c r="J98" s="35"/>
-      <c r="K98" s="35"/>
+    <row r="96" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B96" s="32"/>
+      <c r="C96" s="33"/>
+      <c r="D96" s="33"/>
+      <c r="E96" s="33"/>
+      <c r="F96" s="33"/>
+      <c r="G96" s="33"/>
+      <c r="H96" s="33"/>
+      <c r="I96" s="33"/>
+      <c r="J96" s="33"/>
+      <c r="K96" s="33"/>
+    </row>
+    <row r="98" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="B98" s="68" t="s">
+        <v>185</v>
+      </c>
+      <c r="C98" s="69"/>
+      <c r="D98" s="69"/>
+      <c r="E98" s="69"/>
+      <c r="F98" s="69"/>
+      <c r="G98" s="69"/>
+      <c r="H98" s="69"/>
+      <c r="I98" s="69"/>
+      <c r="J98" s="69"/>
+      <c r="K98" s="69"/>
     </row>
     <row r="99" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B99" s="34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C99" s="35"/>
       <c r="D99" s="35"/>
@@ -2649,7 +2794,7 @@
     </row>
     <row r="100" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B100" s="34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C100" s="35"/>
       <c r="D100" s="35"/>
@@ -2663,7 +2808,7 @@
     </row>
     <row r="101" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B101" s="34" t="s">
-        <v>164</v>
+        <v>31</v>
       </c>
       <c r="C101" s="35"/>
       <c r="D101" s="35"/>
@@ -2677,7 +2822,7 @@
     </row>
     <row r="102" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B102" s="34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C102" s="35"/>
       <c r="D102" s="35"/>
@@ -2691,7 +2836,7 @@
     </row>
     <row r="103" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B103" s="34" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C103" s="35"/>
       <c r="D103" s="35"/>
@@ -2704,7 +2849,9 @@
       <c r="K103" s="35"/>
     </row>
     <row r="104" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B104" s="34"/>
+      <c r="B104" s="34" t="s">
+        <v>160</v>
+      </c>
       <c r="C104" s="35"/>
       <c r="D104" s="35"/>
       <c r="E104" s="35"/>
@@ -2715,63 +2862,482 @@
       <c r="J104" s="35"/>
       <c r="K104" s="35"/>
     </row>
-    <row r="106" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C106" s="71"/>
-      <c r="D106" s="71"/>
-      <c r="E106" s="71"/>
-      <c r="F106" s="71"/>
-      <c r="G106" s="71"/>
-      <c r="H106" s="71"/>
-      <c r="I106" s="71"/>
-      <c r="J106" s="71"/>
-      <c r="K106" s="71"/>
+    <row r="105" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B105" s="34"/>
+      <c r="C105" s="35"/>
+      <c r="D105" s="35"/>
+      <c r="E105" s="35"/>
+      <c r="F105" s="35"/>
+      <c r="G105" s="35"/>
+      <c r="H105" s="35"/>
+      <c r="I105" s="35"/>
+      <c r="J105" s="35"/>
+      <c r="K105" s="35"/>
     </row>
     <row r="107" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C107" s="71"/>
-      <c r="D107" s="71"/>
-      <c r="E107" s="71"/>
-      <c r="F107" s="71"/>
-      <c r="G107" s="71"/>
-      <c r="H107" s="71"/>
-      <c r="I107" s="71"/>
-      <c r="J107" s="71"/>
-      <c r="K107" s="71"/>
+      <c r="B107" s="76"/>
+      <c r="C107" s="76"/>
+      <c r="D107" s="76"/>
+      <c r="E107" s="76"/>
+      <c r="F107" s="76"/>
+      <c r="G107" s="76"/>
+      <c r="H107" s="76"/>
+      <c r="I107" s="76"/>
+      <c r="J107" s="76"/>
+      <c r="K107" s="76"/>
     </row>
     <row r="108" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C108" s="71"/>
-      <c r="D108" s="71"/>
-      <c r="E108" s="71"/>
-      <c r="F108" s="71"/>
-      <c r="G108" s="71"/>
-      <c r="H108" s="71"/>
-      <c r="I108" s="71"/>
-      <c r="J108" s="71"/>
-      <c r="K108" s="71"/>
-    </row>
-    <row r="109" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C109" s="71"/>
-      <c r="D109" s="71"/>
-      <c r="E109" s="71"/>
-      <c r="F109" s="71"/>
-      <c r="G109" s="71"/>
-      <c r="H109" s="71"/>
-      <c r="I109" s="71"/>
-      <c r="J109" s="71"/>
-      <c r="K109" s="71"/>
+      <c r="B108" s="76"/>
+      <c r="C108" s="76"/>
+      <c r="D108" s="76"/>
+      <c r="E108" s="76"/>
+      <c r="F108" s="76"/>
+      <c r="G108" s="76"/>
+      <c r="H108" s="76"/>
+      <c r="I108" s="76"/>
+      <c r="J108" s="76"/>
+      <c r="K108" s="76"/>
+    </row>
+    <row r="109" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="B109" s="77" t="s">
+        <v>225</v>
+      </c>
+      <c r="C109" s="78"/>
+      <c r="D109" s="78"/>
+      <c r="E109" s="78"/>
+      <c r="F109" s="78"/>
+      <c r="G109" s="78"/>
+      <c r="H109" s="78"/>
+      <c r="I109" s="78"/>
+      <c r="J109" s="78"/>
+      <c r="K109" s="78"/>
+    </row>
+    <row r="110" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B110" s="79"/>
+      <c r="C110" s="79"/>
+      <c r="D110" s="79"/>
+      <c r="E110" s="79"/>
+      <c r="F110" s="79"/>
+      <c r="G110" s="79"/>
+      <c r="H110" s="79"/>
+      <c r="I110" s="79"/>
+      <c r="J110" s="79"/>
+      <c r="K110" s="79"/>
+    </row>
+    <row r="111" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B111" s="76"/>
+      <c r="C111" s="80" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="112" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B112" s="76"/>
+      <c r="C112" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="113" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B113" s="76"/>
+    </row>
+    <row r="114" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B114" s="76"/>
+      <c r="C114" s="76" t="s">
+        <v>227</v>
+      </c>
+      <c r="D114" s="76"/>
+      <c r="E114" s="76"/>
+      <c r="F114" s="76"/>
+      <c r="G114" s="76"/>
+      <c r="H114" s="76"/>
+      <c r="I114" s="76"/>
+      <c r="J114" s="76"/>
+      <c r="K114" s="76"/>
+    </row>
+    <row r="115" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B115" s="76"/>
+      <c r="C115" s="76" t="s">
+        <v>226</v>
+      </c>
+      <c r="D115" s="76"/>
+      <c r="E115" s="76"/>
+      <c r="F115" s="76"/>
+      <c r="G115" s="76"/>
+      <c r="H115" s="76"/>
+      <c r="I115" s="76"/>
+      <c r="J115" s="76"/>
+      <c r="K115" s="76"/>
+    </row>
+    <row r="116" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B116" s="76"/>
+    </row>
+    <row r="117" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B117" s="76"/>
+      <c r="C117" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="118" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B118" s="76"/>
+    </row>
+    <row r="119" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B119" s="76"/>
+      <c r="C119" s="76" t="s">
+        <v>200</v>
+      </c>
+      <c r="D119" s="76"/>
+      <c r="E119" s="76"/>
+      <c r="F119" s="76"/>
+      <c r="G119" s="76"/>
+      <c r="H119" s="76"/>
+      <c r="I119" s="76"/>
+      <c r="J119" s="76"/>
+      <c r="K119" s="76"/>
+    </row>
+    <row r="120" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B120" s="76"/>
+    </row>
+    <row r="121" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B121" s="76"/>
+      <c r="C121" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="122" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B122" s="76"/>
+      <c r="C122" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="123" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B123" s="76"/>
+    </row>
+    <row r="124" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B124" s="76"/>
+      <c r="C124" s="76" t="s">
+        <v>203</v>
+      </c>
+      <c r="D124" s="76"/>
+      <c r="E124" s="76"/>
+      <c r="F124" s="76"/>
+      <c r="G124" s="76"/>
+      <c r="H124" s="76"/>
+      <c r="I124" s="76"/>
+      <c r="J124" s="76"/>
+      <c r="K124" s="76"/>
+    </row>
+    <row r="125" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B125" s="76"/>
+    </row>
+    <row r="126" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B126" s="76"/>
+      <c r="C126" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="127" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B127" s="76"/>
+    </row>
+    <row r="128" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B128" s="76"/>
+      <c r="C128" s="76" t="s">
+        <v>205</v>
+      </c>
+      <c r="D128" s="76"/>
+      <c r="E128" s="76"/>
+      <c r="F128" s="76"/>
+      <c r="G128" s="76"/>
+      <c r="H128" s="76"/>
+      <c r="I128" s="76"/>
+      <c r="J128" s="76"/>
+      <c r="K128" s="76"/>
+    </row>
+    <row r="129" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B129" s="76"/>
+    </row>
+    <row r="130" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B130" s="76"/>
+      <c r="C130" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="131" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B131" s="76"/>
+    </row>
+    <row r="132" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B132" s="76"/>
+      <c r="C132" s="76" t="s">
+        <v>207</v>
+      </c>
+      <c r="D132" s="76"/>
+      <c r="E132" s="76"/>
+      <c r="F132" s="76"/>
+      <c r="G132" s="76"/>
+      <c r="H132" s="76"/>
+      <c r="I132" s="76"/>
+      <c r="J132" s="76"/>
+      <c r="K132" s="76"/>
+    </row>
+    <row r="133" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B133" s="76"/>
+      <c r="C133" s="76" t="s">
+        <v>208</v>
+      </c>
+      <c r="D133" s="76"/>
+      <c r="E133" s="76"/>
+      <c r="F133" s="76"/>
+      <c r="G133" s="76"/>
+      <c r="H133" s="76"/>
+      <c r="I133" s="76"/>
+      <c r="J133" s="76"/>
+      <c r="K133" s="76"/>
+    </row>
+    <row r="134" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B134" s="76"/>
+    </row>
+    <row r="135" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B135" s="76"/>
+      <c r="C135" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="136" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B136" s="76"/>
+    </row>
+    <row r="137" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B137" s="76"/>
+      <c r="C137" s="76" t="s">
+        <v>210</v>
+      </c>
+      <c r="D137" s="76"/>
+      <c r="E137" s="76"/>
+      <c r="F137" s="76"/>
+      <c r="G137" s="76"/>
+      <c r="H137" s="76"/>
+      <c r="I137" s="76"/>
+      <c r="J137" s="76"/>
+      <c r="K137" s="76"/>
+    </row>
+    <row r="138" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B138" s="76"/>
+    </row>
+    <row r="139" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B139" s="76"/>
+      <c r="C139" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="140" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B140" s="76"/>
+    </row>
+    <row r="141" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B141" s="76"/>
+      <c r="C141" s="76" t="s">
+        <v>212</v>
+      </c>
+      <c r="D141" s="76"/>
+      <c r="E141" s="76"/>
+      <c r="F141" s="76"/>
+      <c r="G141" s="76"/>
+      <c r="H141" s="76"/>
+      <c r="I141" s="76"/>
+      <c r="J141" s="76"/>
+      <c r="K141" s="76"/>
+    </row>
+    <row r="142" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B142" s="76"/>
+    </row>
+    <row r="143" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B143" s="76"/>
+      <c r="C143" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="144" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B144" s="76"/>
+      <c r="C144" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="145" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B145" s="76"/>
+      <c r="C145" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="146" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B146" s="76"/>
+    </row>
+    <row r="147" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B147" s="76"/>
+      <c r="C147" s="76" t="s">
+        <v>214</v>
+      </c>
+      <c r="D147" s="76"/>
+      <c r="E147" s="76"/>
+      <c r="F147" s="76"/>
+      <c r="G147" s="76"/>
+      <c r="H147" s="76"/>
+      <c r="I147" s="76"/>
+      <c r="J147" s="76"/>
+      <c r="K147" s="76"/>
+    </row>
+    <row r="148" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B148" s="76"/>
+    </row>
+    <row r="149" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B149" s="76"/>
+      <c r="C149" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="150" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B150" s="76"/>
+    </row>
+    <row r="151" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B151" s="76"/>
+      <c r="C151" s="76" t="s">
+        <v>216</v>
+      </c>
+      <c r="D151" s="76"/>
+      <c r="E151" s="76"/>
+      <c r="F151" s="76"/>
+      <c r="G151" s="76"/>
+      <c r="H151" s="76"/>
+      <c r="I151" s="76"/>
+      <c r="J151" s="76"/>
+      <c r="K151" s="76"/>
+    </row>
+    <row r="152" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B152" s="76"/>
+    </row>
+    <row r="153" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B153" s="76"/>
+      <c r="C153" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="154" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B154" s="76"/>
+    </row>
+    <row r="155" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B155" s="76"/>
+      <c r="C155" s="76" t="s">
+        <v>218</v>
+      </c>
+      <c r="D155" s="76"/>
+      <c r="E155" s="76"/>
+      <c r="F155" s="76"/>
+      <c r="G155" s="76"/>
+      <c r="H155" s="76"/>
+      <c r="I155" s="76"/>
+      <c r="J155" s="76"/>
+      <c r="K155" s="76"/>
+    </row>
+    <row r="156" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B156" s="76"/>
+    </row>
+    <row r="157" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B157" s="76"/>
+      <c r="C157" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="158" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B158" s="76"/>
+      <c r="C158" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="159" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B159" s="76"/>
+    </row>
+    <row r="160" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B160" s="76"/>
+      <c r="C160" s="76" t="s">
+        <v>221</v>
+      </c>
+      <c r="D160" s="76"/>
+      <c r="E160" s="76"/>
+      <c r="F160" s="76"/>
+      <c r="G160" s="76"/>
+      <c r="H160" s="76"/>
+      <c r="I160" s="76"/>
+      <c r="J160" s="76"/>
+      <c r="K160" s="76"/>
+    </row>
+    <row r="161" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B161" s="76"/>
+    </row>
+    <row r="162" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B162" s="76"/>
+      <c r="C162" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="163" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B163" s="76"/>
+      <c r="C163" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="164" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B164" s="76"/>
+    </row>
+    <row r="165" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B165" s="76"/>
+      <c r="C165" s="76" t="s">
+        <v>222</v>
+      </c>
+      <c r="D165" s="76"/>
+      <c r="E165" s="76"/>
+      <c r="F165" s="76"/>
+      <c r="G165" s="76"/>
+      <c r="H165" s="76"/>
+      <c r="I165" s="76"/>
+      <c r="J165" s="76"/>
+      <c r="K165" s="76"/>
+    </row>
+    <row r="166" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B166" s="76"/>
+    </row>
+    <row r="167" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B167" s="76"/>
+      <c r="C167" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="168" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B168" s="76"/>
+    </row>
+    <row r="169" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B169" s="76"/>
+      <c r="C169" s="76" t="s">
+        <v>224</v>
+      </c>
+      <c r="D169" s="76"/>
+      <c r="E169" s="76"/>
+      <c r="F169" s="76"/>
+      <c r="G169" s="76"/>
+      <c r="H169" s="76"/>
+      <c r="I169" s="76"/>
+      <c r="J169" s="76"/>
+      <c r="K169" s="76"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B32:K32"/>
-    <mergeCell ref="B51:K51"/>
-    <mergeCell ref="B82:J82"/>
-    <mergeCell ref="B97:K97"/>
-    <mergeCell ref="B83:K83"/>
+  <mergeCells count="13">
+    <mergeCell ref="B109:K109"/>
+    <mergeCell ref="B110:K110"/>
+    <mergeCell ref="B33:K33"/>
+    <mergeCell ref="B52:K52"/>
+    <mergeCell ref="B83:J83"/>
+    <mergeCell ref="B98:K98"/>
     <mergeCell ref="B84:K84"/>
     <mergeCell ref="B85:K85"/>
     <mergeCell ref="B86:K86"/>
     <mergeCell ref="B87:K87"/>
     <mergeCell ref="B88:K88"/>
     <mergeCell ref="B89:K89"/>
+    <mergeCell ref="B90:K90"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2783,486 +3349,563 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:Y1000"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="99" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="224.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="144" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="130.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="25" width="10.5546875" style="1" customWidth="1"/>
-    <col min="26" max="16384" width="11.21875" style="1"/>
+    <col min="1" max="1" width="11.21875" style="1"/>
+    <col min="2" max="2" width="127.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="224.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="144" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="130.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="26" width="10.5546875" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="11.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="81" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="75" t="s">
+    <row r="1" spans="1:26" s="61" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="81" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1" s="55" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="E1" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="F1" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="78" t="s">
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="60"/>
+      <c r="T1" s="60"/>
+      <c r="U1" s="60"/>
+      <c r="V1" s="60"/>
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="60"/>
+    </row>
+    <row r="2" spans="1:26" s="84" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="82">
+        <v>1</v>
+      </c>
+      <c r="B2" s="83" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="79" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="80"/>
-      <c r="Q1" s="80"/>
-      <c r="R1" s="80"/>
-      <c r="S1" s="80"/>
-      <c r="T1" s="80"/>
-      <c r="U1" s="80"/>
-      <c r="V1" s="80"/>
-      <c r="W1" s="80"/>
-      <c r="X1" s="80"/>
-      <c r="Y1" s="80"/>
-    </row>
-    <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="D2" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="E2" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="F2" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="48" t="s">
+    </row>
+    <row r="3" spans="1:26" s="88" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="86">
+        <v>2</v>
+      </c>
+      <c r="B3" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="C3" s="88" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="89" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="47" t="s">
+      <c r="E3" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="F3" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="48" t="s">
+    </row>
+    <row r="4" spans="1:26" s="84" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="82">
+        <v>3</v>
+      </c>
+      <c r="B4" s="90" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="84" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="85" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="E4" s="85" t="s">
+        <v>121</v>
+      </c>
+      <c r="F4" s="85" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" s="88" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="86">
+        <v>4</v>
+      </c>
+      <c r="B5" s="87" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="88" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="89" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="49" t="s">
-        <v>143</v>
-      </c>
-      <c r="C4" s="48" t="s">
+      <c r="E5" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="F5" s="89"/>
+    </row>
+    <row r="6" spans="1:26" s="84" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="82">
+        <v>5</v>
+      </c>
+      <c r="B6" s="90" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="85" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="85" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="85" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" s="88" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="86">
+        <v>6</v>
+      </c>
+      <c r="B7" s="87" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="88" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="89" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="89" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="89" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" s="84" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="82">
+        <v>7</v>
+      </c>
+      <c r="B8" s="83" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="84" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="85" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="85" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" s="88" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="86">
+        <v>8</v>
+      </c>
+      <c r="B9" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="88" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="89" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="89" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="89" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" s="84" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="82">
+        <v>9</v>
+      </c>
+      <c r="B10" s="83" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="85" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="85" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" s="88" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="86">
+        <v>10</v>
+      </c>
+      <c r="B11" s="87" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="88" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="89" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11" s="89" t="s">
         <v>123</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="F11" s="89" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" s="84" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="82">
+        <v>11</v>
+      </c>
+      <c r="B12" s="83" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="84" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="85" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="85" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="85" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" s="88" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="86">
+        <v>12</v>
+      </c>
+      <c r="B13" s="87" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="88" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="89" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="89" t="s">
+        <v>124</v>
+      </c>
+      <c r="F13" s="89" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" s="84" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="82">
+        <v>13</v>
+      </c>
+      <c r="B14" s="83" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="84" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="85" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="85"/>
+      <c r="F14" s="85" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" s="88" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="86">
+        <v>14</v>
+      </c>
+      <c r="B15" s="87" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="88" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="89" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="89" t="s">
+        <v>125</v>
+      </c>
+      <c r="F15" s="89" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="C5" s="48" t="s">
+    <row r="16" spans="1:26" s="84" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="82">
+        <v>15</v>
+      </c>
+      <c r="B16" s="83" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" s="84" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="85" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="85" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="85" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="88" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="86">
+        <v>16</v>
+      </c>
+      <c r="B17" s="87" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="88" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="89" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="89" t="s">
+        <v>126</v>
+      </c>
+      <c r="F17" s="89" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="84" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="82">
+        <v>17</v>
+      </c>
+      <c r="B18" s="83" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="48"/>
-    </row>
-    <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="49" t="s">
-        <v>144</v>
-      </c>
-      <c r="C6" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="48" t="s">
-        <v>124</v>
-      </c>
-      <c r="E6" s="48" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="48" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="48" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="47" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="48" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="48" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="47" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="48" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="47" t="s">
+      <c r="D18" s="85" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" s="85" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="85" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="88" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="86">
+        <v>18</v>
+      </c>
+      <c r="B19" s="87" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="88" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="89" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="89" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" s="89" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="84" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="82">
+        <v>19</v>
+      </c>
+      <c r="B20" s="83" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="84" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="85" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="85" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" s="85" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="88" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="86">
+        <v>20</v>
+      </c>
+      <c r="B21" s="87" t="s">
         <v>111</v>
       </c>
-      <c r="C11" s="48" t="s">
-        <v>115</v>
-      </c>
-      <c r="D11" s="48" t="s">
-        <v>125</v>
-      </c>
-      <c r="E11" s="48" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="47" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="48" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="48" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="48" t="s">
-        <v>116</v>
-      </c>
-      <c r="D13" s="48" t="s">
-        <v>126</v>
-      </c>
-      <c r="E13" s="48" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" s="48" t="s">
+      <c r="C21" s="88" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="89" t="s">
         <v>117</v>
       </c>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="48" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" s="48" t="s">
-        <v>127</v>
-      </c>
-      <c r="E15" s="48" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="47" t="s">
+      <c r="E21" s="89" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="89" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="82">
+        <v>21</v>
+      </c>
+      <c r="B22" s="83" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="84" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="85" t="s">
+        <v>118</v>
+      </c>
+      <c r="E22" s="85" t="s">
+        <v>128</v>
+      </c>
+      <c r="F22" s="85" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="88" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="86">
+        <v>22</v>
+      </c>
+      <c r="B23" s="87" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="88" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="89" t="s">
+        <v>119</v>
+      </c>
+      <c r="E23" s="89" t="s">
+        <v>129</v>
+      </c>
+      <c r="F23" s="89" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="82">
+        <v>23</v>
+      </c>
+      <c r="B24" s="83" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="84" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="85" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="85" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="85" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="88" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="86">
+        <v>24</v>
+      </c>
+      <c r="B25" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="88" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="89" t="s">
+        <v>94</v>
+      </c>
+      <c r="E25" s="89" t="s">
+        <v>95</v>
+      </c>
+      <c r="F25" s="89" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="82">
+        <v>25</v>
+      </c>
+      <c r="B26" s="83" t="s">
         <v>112</v>
       </c>
-      <c r="C16" s="48" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="48" t="s">
-        <v>75</v>
-      </c>
-      <c r="E16" s="48" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="C17" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="D17" s="51" t="s">
-        <v>128</v>
-      </c>
-      <c r="E17" s="51" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="47" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="48" t="s">
-        <v>118</v>
-      </c>
-      <c r="D18" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="48" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="52" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" s="48" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="E19" s="48" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" s="48" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" s="48" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" s="48" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="C21" s="48" t="s">
-        <v>119</v>
-      </c>
-      <c r="D21" s="48" t="s">
-        <v>88</v>
-      </c>
-      <c r="E21" s="48" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" s="48" t="s">
+      <c r="C26" s="83"/>
+      <c r="D26" s="85" t="s">
         <v>120</v>
       </c>
-      <c r="D22" s="48" t="s">
+      <c r="E26" s="85" t="s">
         <v>130</v>
       </c>
-      <c r="E22" s="48" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="C23" s="48" t="s">
-        <v>121</v>
-      </c>
-      <c r="D23" s="48" t="s">
-        <v>131</v>
-      </c>
-      <c r="E23" s="48" t="s">
+      <c r="F26" s="85" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="47" t="s">
-        <v>91</v>
-      </c>
-      <c r="C24" s="48" t="s">
-        <v>92</v>
-      </c>
-      <c r="D24" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="E24" s="48" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="D25" s="48" t="s">
-        <v>97</v>
-      </c>
-      <c r="E25" s="48" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="47" t="s">
-        <v>114</v>
-      </c>
-      <c r="C26" s="48" t="s">
-        <v>122</v>
-      </c>
-      <c r="D26" s="48" t="s">
-        <v>132</v>
-      </c>
-      <c r="E26" s="48" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>